<commit_message>
figured out threading and added second bot, can now run 2 bots at once
</commit_message>
<xml_diff>
--- a/non_code_related_stuff/bots.xlsx
+++ b/non_code_related_stuff/bots.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Brandon\Documents\Personal Projects\twitterContestBot\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Brandon\Documents\Personal Projects\twitterContestBot\non_code_related_stuff\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="41">
   <si>
     <t>gmail</t>
   </si>
@@ -123,13 +123,37 @@
   </si>
   <si>
     <t>bavalley1@cougars.ccis.edu</t>
+  </si>
+  <si>
+    <t>Meow0004</t>
+  </si>
+  <si>
+    <t>doodlebob0045@gmail.com</t>
+  </si>
+  <si>
+    <t>oedC7K7pjmlWtWYvmDQfMWgsY</t>
+  </si>
+  <si>
+    <t>UpN7lmGOfZt2iXNlxaQ3FmtkZO6GjFFDnOq7Y9c5OWBCgEnchY</t>
+  </si>
+  <si>
+    <t>946075554050183169-2VoOR8pk64CBXyjIU04QcnZbfSdxHzn</t>
+  </si>
+  <si>
+    <t>FRouNKabtdALXLpGmSRU4raihlPVkKbm4dmoAk2L6KkDh</t>
+  </si>
+  <si>
+    <t>mobile #</t>
+  </si>
+  <si>
+    <t>1 2185654019</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -147,6 +171,21 @@
       <sz val="8"/>
       <color rgb="FF666666"/>
       <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF66757F"/>
+      <name val="Segoe UI"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -167,10 +206,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -178,8 +218,11 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -458,10 +501,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L6"/>
+  <dimension ref="A1:M7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -471,13 +514,14 @@
     <col min="4" max="4" width="8.77734375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="8.5546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="6.5546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="21.5546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="42.77734375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="41.21875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.77734375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.77734375" customWidth="1"/>
+    <col min="8" max="8" width="21.5546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="42.77734375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="41.21875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>16</v>
       </c>
@@ -497,19 +541,22 @@
         <v>5</v>
       </c>
       <c r="G1" t="s">
+        <v>39</v>
+      </c>
+      <c r="H1" t="s">
         <v>7</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>8</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>31</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
         <v>2</v>
       </c>
@@ -525,20 +572,20 @@
       <c r="F2" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="H2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="I2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="J2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="K2" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="20.399999999999999" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="C3" t="s">
         <v>13</v>
       </c>
@@ -546,20 +593,20 @@
         <v>14</v>
       </c>
       <c r="E3" s="1"/>
-      <c r="G3" s="2" t="s">
+      <c r="H3" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="H3" s="3" t="s">
+      <c r="I3" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="I3" s="2" t="s">
+      <c r="J3" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="J3" s="2" t="s">
+      <c r="K3" s="2" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>15</v>
       </c>
@@ -567,7 +614,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B6" s="4" t="s">
         <v>32</v>
       </c>
@@ -577,27 +624,53 @@
       <c r="D6" t="s">
         <v>23</v>
       </c>
-      <c r="G6" s="2" t="s">
+      <c r="H6" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="H6" s="2" t="s">
+      <c r="I6" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="I6" s="2" t="s">
+      <c r="J6" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="J6" s="2" t="s">
+      <c r="K6" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="K6" t="s">
+      <c r="L6" t="s">
         <v>24</v>
       </c>
-      <c r="L6" t="s">
+      <c r="M6" t="s">
         <v>25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" ht="16.8" x14ac:dyDescent="0.4">
+      <c r="B7" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="D7" t="s">
+        <v>33</v>
+      </c>
+      <c r="G7" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="J7" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="K7" s="2" t="s">
+        <v>38</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B7" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
can now log new users bots follow
</commit_message>
<xml_diff>
--- a/non_code_related_stuff/bots.xlsx
+++ b/non_code_related_stuff/bots.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="45">
   <si>
     <t>gmail</t>
   </si>
@@ -147,6 +147,18 @@
   </si>
   <si>
     <t>1 2185654019</t>
+  </si>
+  <si>
+    <t>bobbybob8005</t>
+  </si>
+  <si>
+    <t>fakepass8005</t>
+  </si>
+  <si>
+    <t>larryjerry220</t>
+  </si>
+  <si>
+    <t>parksandrec</t>
   </si>
 </sst>
 </file>
@@ -501,10 +513,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M7"/>
+  <dimension ref="A1:M9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -666,6 +678,22 @@
         <v>38</v>
       </c>
     </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="B8" t="s">
+        <v>41</v>
+      </c>
+      <c r="D8" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="B9" t="s">
+        <v>43</v>
+      </c>
+      <c r="D9" t="s">
+        <v>44</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B7" r:id="rId1"/>

</xml_diff>